<commit_message>
add cnee code new chage
</commit_message>
<xml_diff>
--- a/public/sample/consignee_bulkimport.xlsx
+++ b/public/sample/consignee_bulkimport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\easemylr-pro\public\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB60FEFE-C49B-4F85-9714-D68A3C5F309D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538F4AD3-9046-4D85-B7BF-C0AC5A182C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F387F7B0-93F9-43D4-9CB3-8572718AEE13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F387F7B0-93F9-43D4-9CB3-8572718AEE13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Sr No.</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Consigner Id</t>
+  </si>
+  <si>
+    <t>Consignee Code</t>
+  </si>
+  <si>
+    <t>code-1011</t>
   </si>
 </sst>
 </file>
@@ -136,6 +142,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -492,20 +499,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D61531-4123-4217-A7F5-85FED5AE74E1}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,52 +523,55 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -571,31 +581,34 @@
       <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>3456789087</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>235742</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{05E36A5B-7606-4A78-89DE-72B3561F6F39}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{05E36A5B-7606-4A78-89DE-72B3561F6F39}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>